<commit_message>
RoleDefinitions and Template Tweaks
</commit_message>
<xml_diff>
--- a/DIGGSRoleDefinitions.xlsx
+++ b/DIGGSRoleDefinitions.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="281">
   <si>
     <t>Code</t>
   </si>
@@ -124,48 +124,9 @@
     <t>time</t>
   </si>
   <si>
-    <t>(amount of substance per time) per area</t>
-  </si>
-  <si>
-    <t>(energy per mass) per time</t>
-  </si>
-  <si>
-    <t>(mass per time) per area</t>
-  </si>
-  <si>
-    <t>(mass per time) per length</t>
-  </si>
-  <si>
-    <t>(mass per volume) per length</t>
-  </si>
-  <si>
-    <t>(volume per time) length</t>
-  </si>
-  <si>
-    <t>(volume per time) per (pressure length)</t>
-  </si>
-  <si>
-    <t>(volume per time) per area</t>
-  </si>
-  <si>
-    <t>(volume per time) per length</t>
-  </si>
-  <si>
-    <t>(volume per time) per pressure</t>
-  </si>
-  <si>
-    <t>(volume per time) per time</t>
-  </si>
-  <si>
-    <t>(volume per time) per volume</t>
-  </si>
-  <si>
     <t>absorbed dose</t>
   </si>
   <si>
-    <t>activity [of radioactivity]</t>
-  </si>
-  <si>
     <t>amount of substance</t>
   </si>
   <si>
@@ -193,15 +154,6 @@
     <t>angular velocity</t>
   </si>
   <si>
-    <t>API gamma ray</t>
-  </si>
-  <si>
-    <t>API gravity</t>
-  </si>
-  <si>
-    <t>API neutron</t>
-  </si>
-  <si>
     <t>area</t>
   </si>
   <si>
@@ -472,9 +424,6 @@
     <t>pressure squared</t>
   </si>
   <si>
-    <t>pressure squared per (force time per area)</t>
-  </si>
-  <si>
     <t>pressure time per volume</t>
   </si>
   <si>
@@ -487,9 +436,6 @@
     <t>radiant intensity</t>
   </si>
   <si>
-    <t>reciprocal (mass time)</t>
-  </si>
-  <si>
     <t>reciprocal area</t>
   </si>
   <si>
@@ -685,15 +631,6 @@
     <t>token</t>
   </si>
   <si>
-    <t>reciprocal square root time</t>
-  </si>
-  <si>
-    <t>reciprocal time (per time)</t>
-  </si>
-  <si>
-    <t>rolePerformed</t>
-  </si>
-  <si>
     <t>Operator</t>
   </si>
   <si>
@@ -854,6 +791,93 @@
   </si>
   <si>
     <t>DIGGS_Roles</t>
+  </si>
+  <si>
+    <t>activity of radioactivity</t>
+  </si>
+  <si>
+    <t>amount of substance per time per area</t>
+  </si>
+  <si>
+    <t>api gamma ray</t>
+  </si>
+  <si>
+    <t>api gravity</t>
+  </si>
+  <si>
+    <t>api neutron</t>
+  </si>
+  <si>
+    <t>area per count</t>
+  </si>
+  <si>
+    <t>cation exchange capacity</t>
+  </si>
+  <si>
+    <t>density or unit weight</t>
+  </si>
+  <si>
+    <t>diffusive time of flight</t>
+  </si>
+  <si>
+    <t>energy per mass per time</t>
+  </si>
+  <si>
+    <t>mass per time per area</t>
+  </si>
+  <si>
+    <t>mass per time per length</t>
+  </si>
+  <si>
+    <t>mass per volume per length</t>
+  </si>
+  <si>
+    <t>mass per volume per pressure</t>
+  </si>
+  <si>
+    <t>mass per volume per temperature</t>
+  </si>
+  <si>
+    <t>pressure per pressure</t>
+  </si>
+  <si>
+    <t>pressure squared per force time per area</t>
+  </si>
+  <si>
+    <t>reciprocal mass time</t>
+  </si>
+  <si>
+    <t>reciprocal time squared</t>
+  </si>
+  <si>
+    <t>thermodynamic temperature per thermodynamic temperature</t>
+  </si>
+  <si>
+    <t>unitless</t>
+  </si>
+  <si>
+    <t>vertical coordinate</t>
+  </si>
+  <si>
+    <t>volume per time length</t>
+  </si>
+  <si>
+    <t>volume per time per area</t>
+  </si>
+  <si>
+    <t>volume per time per length</t>
+  </si>
+  <si>
+    <t>volume per time per pressure</t>
+  </si>
+  <si>
+    <t>volume per time per pressure length</t>
+  </si>
+  <si>
+    <t>volume per time per time</t>
+  </si>
+  <si>
+    <t>volume per time per volume</t>
   </si>
 </sst>
 </file>
@@ -1216,8 +1240,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C178" totalsRowShown="0">
-  <autoFilter ref="A1:C178"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:C187" totalsRowShown="0">
+  <autoFilter ref="A1:C187"/>
   <sortState ref="A2:C178">
     <sortCondition ref="C1:C178"/>
   </sortState>
@@ -1496,7 +1520,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1512,7 +1536,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>16</v>
@@ -1521,39 +1545,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="3"/>
+    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="2"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A3" s="4"/>
       <c r="B3" s="3" t="s">
-        <v>272</v>
+        <v>251</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>271</v>
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.5">
       <c r="C13" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.5">
       <c r="D14" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D17" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="4:4" x14ac:dyDescent="0.5">
       <c r="D19" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1571,7 +1598,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1592,7 +1619,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>265</v>
+        <v>244</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -1604,7 +1631,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -1619,26 +1646,26 @@
         <v/>
       </c>
       <c r="B2" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C2" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>operator</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1647,26 +1674,24 @@
         <v/>
       </c>
       <c r="B3" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C3" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>logger</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G3" s="4"/>
       <c r="H3" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1675,26 +1700,24 @@
         <v/>
       </c>
       <c r="B4" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C4" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>drilling_contractor</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>224</v>
+        <v>203</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G4" s="4"/>
       <c r="H4" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1703,26 +1726,24 @@
         <v/>
       </c>
       <c r="B5" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C5" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>insitu_contractor</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G5" s="4"/>
       <c r="H5" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1731,26 +1752,24 @@
         <v/>
       </c>
       <c r="B6" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C6" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>laboratory_name</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>227</v>
+        <v>206</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1759,26 +1778,24 @@
         <v/>
       </c>
       <c r="B7" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C7" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>project_engineer</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>228</v>
+        <v>207</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>229</v>
+        <v>208</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G7" s="4"/>
       <c r="H7" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1787,26 +1804,24 @@
         <v/>
       </c>
       <c r="B8" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C8" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>project_manager</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>230</v>
+        <v>209</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1815,26 +1830,24 @@
         <v/>
       </c>
       <c r="B9" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C9" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>checked_by</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>232</v>
+        <v>211</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>233</v>
+        <v>212</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G9" s="4"/>
       <c r="H9" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1843,26 +1856,24 @@
         <v/>
       </c>
       <c r="B10" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C10" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>prepared_by</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>234</v>
+        <v>213</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>235</v>
+        <v>214</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G10" s="4"/>
       <c r="H10" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1871,26 +1882,24 @@
         <v/>
       </c>
       <c r="B11" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C11" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>calculated_by</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>236</v>
+        <v>215</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>237</v>
+        <v>216</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G11" s="4"/>
       <c r="H11" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1899,26 +1908,24 @@
         <v/>
       </c>
       <c r="B12" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C12" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>tested_by</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>238</v>
+        <v>217</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G12" s="4"/>
       <c r="H12" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1927,26 +1934,24 @@
         <v/>
       </c>
       <c r="B13" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C13" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>owner</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>239</v>
+        <v>218</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>240</v>
+        <v>219</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G13" s="4"/>
       <c r="H13" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1955,26 +1960,24 @@
         <v/>
       </c>
       <c r="B14" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C14" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>client</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>241</v>
+        <v>220</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G14" s="4"/>
       <c r="H14" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.5">
@@ -1983,26 +1986,24 @@
         <v/>
       </c>
       <c r="B15" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="C15" s="10" t="str">
         <f>SUBSTITUTE(SUBSTITUTE(LOWER(Definitions[[#This Row],[Name]])," ","_"),"/","_")</f>
         <v>helper</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="4" t="s">
-        <v>12</v>
-      </c>
+      <c r="G15" s="4"/>
       <c r="H15" s="3" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2043,7 +2044,7 @@
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2070,10 +2071,10 @@
         <v/>
       </c>
       <c r="B2" s="10" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
@@ -2082,10 +2083,10 @@
         <v/>
       </c>
       <c r="B3" s="10" t="s">
-        <v>249</v>
+        <v>228</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
@@ -2094,10 +2095,10 @@
         <v/>
       </c>
       <c r="B4" s="10" t="s">
-        <v>250</v>
+        <v>229</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
@@ -2106,10 +2107,10 @@
         <v/>
       </c>
       <c r="B5" s="10" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
@@ -2118,10 +2119,10 @@
         <v/>
       </c>
       <c r="B6" s="10" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
@@ -2130,10 +2131,10 @@
         <v/>
       </c>
       <c r="B7" s="10" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
@@ -2142,10 +2143,10 @@
         <v/>
       </c>
       <c r="B8" s="10" t="s">
-        <v>254</v>
+        <v>233</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
@@ -2154,10 +2155,10 @@
         <v/>
       </c>
       <c r="B9" s="10" t="s">
-        <v>255</v>
+        <v>234</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
@@ -2166,10 +2167,10 @@
         <v/>
       </c>
       <c r="B10" s="10" t="s">
-        <v>256</v>
+        <v>235</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
@@ -2178,10 +2179,10 @@
         <v/>
       </c>
       <c r="B11" s="10" t="s">
-        <v>257</v>
+        <v>236</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
@@ -2190,10 +2191,10 @@
         <v/>
       </c>
       <c r="B12" s="10" t="s">
-        <v>258</v>
+        <v>237</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
@@ -2202,10 +2203,10 @@
         <v/>
       </c>
       <c r="B13" s="10" t="s">
-        <v>259</v>
+        <v>238</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
@@ -2214,10 +2215,10 @@
         <v/>
       </c>
       <c r="B14" s="10" t="s">
-        <v>260</v>
+        <v>239</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>263</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
@@ -2226,10 +2227,10 @@
         <v/>
       </c>
       <c r="B15" s="10" t="s">
-        <v>261</v>
+        <v>240</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>262</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -2248,10 +2249,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:C178"/>
+  <dimension ref="A1:C187"/>
   <sheetViews>
-    <sheetView topLeftCell="A166" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A181" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C154" sqref="C154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2265,15 +2266,15 @@
         <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>187</v>
+        <v>169</v>
       </c>
       <c r="C1" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B2" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="C2" t="s">
         <v>29</v>
@@ -2281,50 +2282,50 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
-        <v>197</v>
+        <v>179</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
-        <v>196</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
-        <v>211</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
-        <v>189</v>
+        <v>171</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
@@ -2332,71 +2333,71 @@
         <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
-        <v>194</v>
+        <v>176</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
-        <v>195</v>
+        <v>177</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
-        <v>193</v>
+        <v>175</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
-        <v>192</v>
+        <v>174</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>255</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B17" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="C17" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.5">
@@ -2404,71 +2405,71 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B19" t="s">
-        <v>202</v>
+        <v>184</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B20" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="C20" t="s">
-        <v>47</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B21" t="s">
-        <v>206</v>
+        <v>188</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B22" t="s">
-        <v>205</v>
+        <v>187</v>
       </c>
       <c r="C22" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B23" t="s">
-        <v>203</v>
+        <v>185</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B24" t="s">
-        <v>214</v>
+        <v>196</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B25" t="s">
-        <v>208</v>
+        <v>190</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B26" t="s">
-        <v>209</v>
+        <v>191</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>258</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.5">
@@ -2476,7 +2477,7 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.5">
@@ -2484,692 +2485,692 @@
         <v>28</v>
       </c>
       <c r="C28" t="s">
-        <v>55</v>
+        <v>259</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B29" t="s">
-        <v>215</v>
+        <v>197</v>
       </c>
       <c r="C29" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B30" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="C30" t="s">
-        <v>57</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B31" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="C31" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B32" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.5">
       <c r="B33" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C34" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C35" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C36" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C37" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C38" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C39" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C40" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C41" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C42" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C43" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C44" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C45" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C46" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C47" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.5">
       <c r="C48" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="49" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C49" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="50" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C50" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="51" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C51" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C52" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C53" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C54" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
     </row>
     <row r="55" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C55" t="s">
-        <v>23</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C56" t="s">
-        <v>78</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C57" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="58" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C58" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C59" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="60" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C60" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="61" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C61" t="s">
-        <v>83</v>
+        <v>21</v>
       </c>
     </row>
     <row r="62" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C62" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="63" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C63" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C64" t="s">
-        <v>7</v>
+        <v>73</v>
       </c>
     </row>
     <row r="65" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C65" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C66" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C67" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C68" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C69" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C70" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="71" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C71" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="72" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C72" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="73" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C73" t="s">
-        <v>92</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C74" t="s">
-        <v>93</v>
+        <v>22</v>
       </c>
     </row>
     <row r="75" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C75" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="76" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C76" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C77" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C78" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
     </row>
     <row r="79" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C79" t="s">
-        <v>4</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C80" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C81" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C82" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C83" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C84" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
     </row>
     <row r="85" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C85" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
     </row>
     <row r="86" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C86" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="87" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C87" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="88" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C88" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="89" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C89" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C90" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="91" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C91" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C92" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="93" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C93" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
     </row>
     <row r="94" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C94" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="95" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C95" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="96" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C96" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="97" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C97" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C98" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="99" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C99" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C100" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="101" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C101" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="102" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C102" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
     </row>
     <row r="103" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C103" t="s">
-        <v>119</v>
+        <v>262</v>
       </c>
     </row>
     <row r="104" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C104" t="s">
-        <v>120</v>
+        <v>263</v>
       </c>
     </row>
     <row r="105" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C105" t="s">
-        <v>121</v>
+        <v>20</v>
       </c>
     </row>
     <row r="106" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C106" t="s">
-        <v>122</v>
+        <v>264</v>
       </c>
     </row>
     <row r="107" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C107" t="s">
-        <v>123</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C108" t="s">
-        <v>124</v>
+        <v>266</v>
       </c>
     </row>
     <row r="109" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C109" t="s">
-        <v>20</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C110" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C111" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C112" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C113" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C114" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C115" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C116" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C117" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C118" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C119" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C120" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C121" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
     </row>
     <row r="122" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C122" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C123" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C124" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="125" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C125" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C126" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
     </row>
     <row r="127" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C127" t="s">
-        <v>141</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C128" t="s">
-        <v>5</v>
+        <v>267</v>
       </c>
     </row>
     <row r="129" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C129" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
     </row>
     <row r="130" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C130" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="131" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C131" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
     </row>
     <row r="132" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C132" t="s">
-        <v>145</v>
+        <v>268</v>
       </c>
     </row>
     <row r="133" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C133" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C134" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C135" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C136" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C137" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C138" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C139" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C140" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
     </row>
     <row r="141" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C141" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
     </row>
     <row r="142" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C142" t="s">
-        <v>155</v>
+        <v>269</v>
       </c>
     </row>
     <row r="143" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C143" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="144" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C144" t="s">
-        <v>216</v>
+        <v>139</v>
       </c>
     </row>
     <row r="145" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C145" t="s">
-        <v>157</v>
+        <v>270</v>
       </c>
     </row>
     <row r="146" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C146" t="s">
-        <v>217</v>
+        <v>140</v>
       </c>
     </row>
     <row r="147" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C147" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
     </row>
     <row r="148" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C148" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
     </row>
     <row r="149" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C149" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
     </row>
     <row r="150" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C150" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
     </row>
     <row r="151" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C151" t="s">
-        <v>162</v>
+        <v>145</v>
       </c>
     </row>
     <row r="152" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C152" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
     </row>
     <row r="153" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C153" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="154" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C154" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
     </row>
     <row r="155" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C155" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
     </row>
     <row r="156" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C156" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
     </row>
     <row r="157" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C157" t="s">
-        <v>168</v>
+        <v>151</v>
       </c>
     </row>
     <row r="158" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C158" t="s">
-        <v>169</v>
+        <v>152</v>
       </c>
     </row>
     <row r="159" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C159" t="s">
-        <v>170</v>
+        <v>153</v>
       </c>
     </row>
     <row r="160" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C160" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
     </row>
     <row r="161" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C161" t="s">
-        <v>172</v>
+        <v>25</v>
       </c>
     </row>
     <row r="162" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C162" t="s">
-        <v>25</v>
+        <v>271</v>
       </c>
     </row>
     <row r="163" spans="3:3" x14ac:dyDescent="0.5">
@@ -3184,72 +3185,117 @@
     </row>
     <row r="165" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C165" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
     </row>
     <row r="166" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C166" t="s">
-        <v>174</v>
+        <v>156</v>
       </c>
     </row>
     <row r="167" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C167" t="s">
-        <v>175</v>
+        <v>157</v>
       </c>
     </row>
     <row r="168" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C168" t="s">
-        <v>176</v>
+        <v>272</v>
       </c>
     </row>
     <row r="169" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C169" t="s">
-        <v>177</v>
+        <v>273</v>
       </c>
     </row>
     <row r="170" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C170" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
     </row>
     <row r="171" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C171" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
     </row>
     <row r="172" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C172" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
     </row>
     <row r="173" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C173" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
     </row>
     <row r="174" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C174" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="175" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C175" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
     </row>
     <row r="176" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C176" t="s">
-        <v>14</v>
+        <v>164</v>
       </c>
     </row>
     <row r="177" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C177" t="s">
-        <v>184</v>
+        <v>165</v>
       </c>
     </row>
     <row r="178" spans="3:3" x14ac:dyDescent="0.5">
       <c r="C178" t="s">
-        <v>185</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C179" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C180" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C181" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C182" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C183" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C184" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C185" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C186" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.5">
+      <c r="C187" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>